<commit_message>
Fixed tests with more verbose errors for import; Increased verbosity of errors during uploading; Fixes #30
</commit_message>
<xml_diff>
--- a/castoredc_api/tests/test_import/data_files_for_import_tests/data_file_report_medication_final_errors.xlsx
+++ b/castoredc_api/tests/test_import/data_files_for_import_tests/data_file_report_medication_final_errors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>110001</t>
   </si>
@@ -79,10 +79,13 @@
     <t>med_other_unit</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>Error: unprocessable date</t>
+  </si>
+  <si>
+    <t>Error: not a number</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,16 +484,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
@@ -504,16 +507,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
@@ -527,16 +530,16 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
@@ -550,16 +553,16 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>9</v>
@@ -573,16 +576,16 @@
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>13</v>

</xml_diff>